<commit_message>
primera version calculo creditos; no valida
No valida al no contar desdobles de grupos!
Se debe usar otra fuente de datos...
</commit_message>
<xml_diff>
--- a/asignaturas_ingmec.xlsx
+++ b/asignaturas_ingmec.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428D929-720E-4280-8853-0D024F1E4BFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727880A6-2633-40B5-9C52-E15B42FBEC23}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" tabRatio="467" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="asignaturas_profesores" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">asignaturas_profesores!$A$1:$C$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">asignaturas_profesores!$A$1:$C$86</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="135">
   <si>
     <t>Expresión Gráfica</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Neumática y Oleohidráulica</t>
   </si>
   <si>
-    <t>Prácticas Externas en Empresa</t>
-  </si>
-  <si>
     <t>Cálculo y Diseño de Máquinas II</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>Oficina Técnica y Proyectos</t>
   </si>
   <si>
-    <t>Trabajo Fin de Grado</t>
-  </si>
-  <si>
     <t>codigo</t>
   </si>
   <si>
@@ -160,9 +154,6 @@
     <t>creditos</t>
   </si>
   <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
     <t>área</t>
   </si>
   <si>
@@ -208,12 +199,6 @@
     <t>Profesor5</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jiménez Guerrero, José Felipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Plaza Úbeda, José Antonio</t>
-  </si>
-  <si>
     <t>Galera Quiles, María del Carmen</t>
   </si>
   <si>
@@ -226,42 +211,24 @@
     <t>Sánchez Pérez, José Antonio</t>
   </si>
   <si>
-    <t xml:space="preserve"> Miralles Cuevas, Sara</t>
-  </si>
-  <si>
     <t>Física Aplicada</t>
   </si>
   <si>
     <t>Posadas Chinchilla, Antonio Miguel</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nieves López, Francisco Javier de las</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pérez García, Manuel</t>
-  </si>
-  <si>
     <t>Estadística e Investigación Operativa</t>
   </si>
   <si>
     <t xml:space="preserve"> Martínez López, Ignacio Jesús</t>
   </si>
   <si>
-    <t xml:space="preserve"> Juan González, Alicia María</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Martínez Puertas, Sergio</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Oña Casado, Inmaculada</t>
   </si>
   <si>
     <t>Corchete Fernández, Víctor</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fernández Barbero, Antonio José</t>
-  </si>
-  <si>
     <t>Matemática Aplicada</t>
   </si>
   <si>
@@ -280,24 +247,12 @@
     <t>García Lázaro, José Rafael</t>
   </si>
   <si>
-    <t xml:space="preserve"> Guirado Clavijo, Rafael</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aguila Cano, Isabel María del</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Becerra Terón, Antonio</t>
   </si>
   <si>
-    <t xml:space="preserve"> López Martínez, Alejandro</t>
-  </si>
-  <si>
     <t>Martínez Lao, Juan Antonio</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gómez Galán, Marta</t>
-  </si>
-  <si>
     <t>Andújar Rodríguez, Antonio Serafín</t>
   </si>
   <si>
@@ -389,13 +344,97 @@
   </si>
   <si>
     <t>García Buendía, Antonio</t>
+  </si>
+  <si>
+    <t>Aguilar Torres, Manuel Angel</t>
+  </si>
+  <si>
+    <t>González Yebra, Óscar</t>
+  </si>
+  <si>
+    <t>Aguilar Torres, Fernando José</t>
+  </si>
+  <si>
+    <t>Garzón Garzón, Eduardo</t>
+  </si>
+  <si>
+    <t>Díaz Pérez, Manuel</t>
+  </si>
+  <si>
+    <t>López Martínez, José Antonio</t>
+  </si>
+  <si>
+    <t>López Martínez, Alejandro</t>
+  </si>
+  <si>
+    <t>Callejón Ferre, Ángel Jesús</t>
+  </si>
+  <si>
+    <t>Garrido Jiménez, Francisco Javier</t>
+  </si>
+  <si>
+    <t>Ramos Teodoro, Jerónimo</t>
+  </si>
+  <si>
+    <t>Fernández Ros, Manuel</t>
+  </si>
+  <si>
+    <t>Gázquez Parra, José Antonio</t>
+  </si>
+  <si>
+    <t>López Ramos, Juan Antonio</t>
+  </si>
+  <si>
+    <t>Lirola Terrez, Antonio</t>
+  </si>
+  <si>
+    <t>Escoriza López, José</t>
+  </si>
+  <si>
+    <t>Cuadra Díaz, Juan</t>
+  </si>
+  <si>
+    <t>Pérez Castro, Agustín</t>
+  </si>
+  <si>
+    <t>Juan González, Alicia María</t>
+  </si>
+  <si>
+    <t>Nieves López, Francisco Javier de las</t>
+  </si>
+  <si>
+    <t>Fernández Barbero, Antonio José</t>
+  </si>
+  <si>
+    <t>Guirado Clavijo, Rafael</t>
+  </si>
+  <si>
+    <t>Plaza Úbeda, José Antonio</t>
+  </si>
+  <si>
+    <t>Miralles Cuevas, Sara</t>
+  </si>
+  <si>
+    <t>Gómez Galán, Marta</t>
+  </si>
+  <si>
+    <t>Aguila Cano, Isabel María del</t>
+  </si>
+  <si>
+    <t>Martínez Puertas, Sergio</t>
+  </si>
+  <si>
+    <t>Pérez García, Manuel</t>
+  </si>
+  <si>
+    <t>Jiménez Guerrero, José Felipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,13 +442,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -424,9 +477,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,48 +797,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
     <col min="5" max="9" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -796,7 +852,19 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -810,7 +878,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -824,7 +898,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -838,7 +915,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -852,7 +935,13 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -866,7 +955,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -880,7 +972,13 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -894,7 +992,10 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -902,13 +1003,16 @@
         <v>29104213</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -916,13 +1020,22 @@
         <v>29104218</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -930,13 +1043,19 @@
         <v>29104219</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,13 +1063,16 @@
         <v>29104221</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -958,286 +1080,337 @@
         <v>29104223</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>29104224</v>
+        <v>43103215</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>29104227</v>
+        <v>43103220</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>43103215</v>
+        <v>43104213</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>43103220</v>
+        <v>44101101</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>43104213</v>
+        <v>44101102</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>44101101</v>
+        <v>44101103</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>44101102</v>
+        <v>44101105</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>44101103</v>
+        <v>44101106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>44101105</v>
+        <v>44101107</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>131</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>44101106</v>
+        <v>44101108</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>61</v>
+      </c>
+      <c r="G24" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>44101107</v>
+        <v>44101109</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>44101108</v>
+        <v>44101110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>44101109</v>
+        <v>44101209</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>44101110</v>
+        <v>44102104</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>44101209</v>
+        <v>44102201</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -1246,21 +1419,21 @@
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>44102104</v>
+        <v>44102202</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -1269,287 +1442,247 @@
         <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="F30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>44102201</v>
+        <v>44102203</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>44102202</v>
+        <v>44102204</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>85</v>
+      </c>
+      <c r="G32" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>44102203</v>
+        <v>44102205</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>44102204</v>
+        <v>44102206</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C34">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>44102205</v>
+        <v>44102207</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="G35" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>44102206</v>
+        <v>44102208</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>44102207</v>
+        <v>44102211</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>44102208</v>
+        <v>44103216</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C38">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>44102211</v>
+        <v>44103217</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>110</v>
-      </c>
-      <c r="F39" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>44103216</v>
+        <v>44103223</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>44103217</v>
+        <v>44104210</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>44103223</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
         <v>102</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F41" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>44104210</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" t="s">
-        <v>117</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45">
-        <f>SUM(C2:C44)</f>
-        <v>264</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
     </row>
@@ -1654,15 +1787,6 @@
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>